<commit_message>
Don't know what I updated here
</commit_message>
<xml_diff>
--- a/Book4.xlsx
+++ b/Book4.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://streamrealty-my.sharepoint.com/personal/jgilles_streamdatacenters_com/Documents/Documents/GitHub/baker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2696" documentId="8_{0EA9A5FB-C638-4B36-B461-94A22AD010CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F9C18F5-A0F6-4481-AF49-41BF6BCDDF91}"/>
+  <xr:revisionPtr revIDLastSave="2844" documentId="8_{0EA9A5FB-C638-4B36-B461-94A22AD010CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D53DAC3-9C9C-4455-8026-783439D37C86}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F613AA21-5772-4279-AB7F-8475EF583609}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{F613AA21-5772-4279-AB7F-8475EF583609}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet7" sheetId="7" r:id="rId1"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId1"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="244">
   <si>
     <t>4h</t>
   </si>
@@ -712,6 +713,90 @@
   </si>
   <si>
     <t>Change non-column to column if needed / helpful</t>
+  </si>
+  <si>
+    <t>Options for each move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Move onto the timeline (T), </t>
+  </si>
+  <si>
+    <t>Maybe ins</t>
+  </si>
+  <si>
+    <t>timeline</t>
+  </si>
+  <si>
+    <t>foundation</t>
+  </si>
+  <si>
+    <t>uncovered</t>
+  </si>
+  <si>
+    <t>covered</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Source State</t>
+  </si>
+  <si>
+    <t>Desintation State</t>
+  </si>
+  <si>
+    <t>Check higher card for move to foundation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lock card = blue </t>
+  </si>
+  <si>
+    <t>Check parent for foundation. Make parent uncoverd.</t>
+  </si>
+  <si>
+    <t>Gets covered with Lower.</t>
+  </si>
+  <si>
+    <t>Timeline lock releases only when Higher is moved to timeline or uncoverd</t>
+  </si>
+  <si>
+    <t>When Child is moved. Releases Higher Lock</t>
+  </si>
+  <si>
+    <t>Always locked.</t>
+  </si>
+  <si>
+    <t>Avaliable card</t>
+  </si>
+  <si>
+    <t>When lock changes avalibility should also change</t>
+  </si>
+  <si>
+    <t>false means passed on moving timeline to uncovered. Has the same effect as locking the card</t>
+  </si>
+  <si>
+    <t>always false</t>
+  </si>
+  <si>
+    <t>false means passed on moving to timeline, has same effect as locking and same release condiiton.</t>
+  </si>
+  <si>
+    <t>This is not actually needed as it appears placing a lock performs the same function</t>
+  </si>
+  <si>
+    <t>Lower is going directly on top</t>
+  </si>
+  <si>
+    <t>*Only called when Lower is moving onto Higher</t>
+  </si>
+  <si>
+    <t>Uncovered lock releases only when timeline has been filled.</t>
+  </si>
+  <si>
+    <t>Move onto Higher, update Higher to be covered.</t>
+  </si>
+  <si>
+    <t>Move onto Higher, update Higher to be covered. Update Parent to be uncovered</t>
   </si>
 </sst>
 </file>
@@ -876,7 +961,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -987,6 +1072,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4547,11 +4647,165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99085223-FA2E-4344-88FD-02D01ED8E221}">
+  <dimension ref="A2:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="20.7109375" style="43" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="43" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="43" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>220</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>225</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="43" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="43" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B7" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="F7" s="46" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B9" s="44" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B10" s="43" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B11" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>236</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>236</v>
+      </c>
+      <c r="F11" s="43" t="s">
+        <v>237</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0A8E39-78E8-4D70-A478-95B4D5C25058}">
-  <dimension ref="B2:Q40"/>
+  <dimension ref="B2:Q45"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4872,6 +5126,21 @@
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -4893,12 +5162,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B2471E-03CC-4858-8E0E-8CCCB4CE99F2}">
   <dimension ref="B1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6018,7 +6287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3DAFA7-884A-4444-8935-39B37507A7F9}">
   <dimension ref="B2:V19"/>
   <sheetViews>
@@ -6163,7 +6432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE25AD15-5806-40AC-A954-4B4CB9E2F599}">
   <dimension ref="A1:S32"/>
   <sheetViews>
@@ -6858,7 +7127,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDDD59F9-8970-4CCB-A1B1-62B2ABC0F859}">
   <dimension ref="A1:W23"/>
   <sheetViews>
@@ -6879,28 +7148,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
       <c r="W1" t="s">
         <v>106</v>
       </c>
@@ -7344,28 +7613,28 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C10" s="16"/>
@@ -7782,28 +8051,28 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
-      <c r="N17" s="44"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44"/>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="44"/>
-      <c r="S17" s="44"/>
-      <c r="T17" s="44"/>
-      <c r="U17" s="44"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+      <c r="U17" s="49"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C18" s="16"/>
@@ -8229,7 +8498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78E2845-6DB6-47AE-B661-265E49538383}">
   <dimension ref="A1:AA16"/>
   <sheetViews>
@@ -8262,21 +8531,21 @@
       <c r="F1" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
       <c r="V1" s="20" t="s">
         <v>98</v>
       </c>
@@ -9274,7 +9543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B555979D-2A3C-4A6C-BD66-3CC5DE6E8ED3}">
   <dimension ref="B2:BN45"/>
   <sheetViews>

</xml_diff>